<commit_message>
falsche Excel Tabelle mit Darstellung der Einrichtungen korrigiert
</commit_message>
<xml_diff>
--- a/Ergebnisse/Excel/Einrichtungen/Sbbz_Hze.xlsx
+++ b/Ergebnisse/Excel/Einrichtungen/Sbbz_Hze.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Einrichtung</t>
   </si>
@@ -26,72 +26,27 @@
     <t xml:space="preserve">Jugendhilfeverbund Kinderheim Rodt</t>
   </si>
   <si>
-    <t xml:space="preserve">9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ev Jugendhilfe Heilbronn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19</t>
+    <t xml:space="preserve">Ev Jugendhilfe Friedenshort</t>
   </si>
   <si>
     <t xml:space="preserve">Jugendhilfe Hoffmannhaus Wilhelmsdorf</t>
   </si>
   <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stiftung Jugendhilfe aktiv Region Stuttgart</t>
+    <t xml:space="preserve">Stiftung Jugendhilfe aktiv</t>
   </si>
   <si>
     <t xml:space="preserve">Jugendhilfe Hochdorf</t>
   </si>
   <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sophienpflege Tübingen</t>
   </si>
   <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Stiftung Tragwerk KirchheimTeck</t>
   </si>
   <si>
-    <t xml:space="preserve">17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stiftung Jugendhilfe aktiv Region Böblingen</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mutpol Tuttlingen</t>
   </si>
   <si>
-    <t xml:space="preserve">23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stiftung Jugendhilfe aktiv Region Esslingen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
     <t xml:space="preserve">eva Heidenheim</t>
   </si>
   <si>
@@ -104,9 +59,6 @@
     <t xml:space="preserve">Jugendhilfe Korntal</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Johannes_Falk_Haus Stuttgart</t>
   </si>
   <si>
@@ -116,21 +68,12 @@
     <t xml:space="preserve">Jugendhilfeverbund Paulinenpflege Winnenden</t>
   </si>
   <si>
-    <t xml:space="preserve">22</t>
-  </si>
-  <si>
     <t xml:space="preserve">Diakonische Jugendhilfe Heilbronn (DJHN)</t>
   </si>
   <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
     <t xml:space="preserve">eva Stuttgart</t>
   </si>
   <si>
-    <t xml:space="preserve">40</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mariaberger Heime Gammertingen</t>
   </si>
   <si>
@@ -138,9 +81,6 @@
   </si>
   <si>
     <t xml:space="preserve">Diasporahaus Bietenhausen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
   </si>
   <si>
     <t xml:space="preserve">Weraheim Hebsack</t>
@@ -493,264 +433,242 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
+      <c r="B2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C2" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4" t="n">
         <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
+        <v>8</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B9" t="n">
+        <v>23</v>
+      </c>
+      <c r="C9" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
+        <v>11</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>34</v>
+        <v>19</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" t="s">
-        <v>36</v>
+        <v>20</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" t="s">
-        <v>38</v>
+        <v>21</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
+        <v>22</v>
+      </c>
+      <c r="B21" t="n">
+        <v>15</v>
+      </c>
+      <c r="C21" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
+        <v>23</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
         <v>4</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Leitung als Spalte in Versuchspersonen nach Einrichtung ergänzt
</commit_message>
<xml_diff>
--- a/Ergebnisse/Excel/Einrichtungen/Sbbz_Hze.xlsx
+++ b/Ergebnisse/Excel/Einrichtungen/Sbbz_Hze.xlsx
@@ -12,9 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">Einrichtung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leitung</t>
   </si>
   <si>
     <t xml:space="preserve">SBBZ</t>
@@ -428,246 +431,315 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="n">
         <v>3</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>9</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C3" t="n">
         <v>4</v>
       </c>
-      <c r="B3" t="n">
-        <v>4</v>
-      </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="n">
         <v>6</v>
       </c>
       <c r="C4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="n">
+        <v>12</v>
+      </c>
+      <c r="C5" t="n">
         <v>6</v>
       </c>
-      <c r="B5" t="n">
-        <v>6</v>
-      </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" t="n">
         <v>2</v>
       </c>
       <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" t="n">
         <v>23</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
         <v>1</v>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
       </c>
       <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" t="n">
         <v>1</v>
       </c>
-      <c r="C15" t="n">
+      <c r="D15" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B19" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" t="n">
         <v>1</v>
       </c>
-      <c r="C19" t="n">
+      <c r="D19" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B21" t="n">
+        <v>5</v>
+      </c>
+      <c r="C21" t="n">
         <v>15</v>
       </c>
-      <c r="C21" t="n">
+      <c r="D21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Start mit Auswertung nach Einrichtungen
</commit_message>
<xml_diff>
--- a/Ergebnisse/Excel/Einrichtungen/Sbbz_Hze.xlsx
+++ b/Ergebnisse/Excel/Einrichtungen/Sbbz_Hze.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">Einrichtung</t>
   </si>
@@ -35,7 +35,7 @@
     <t xml:space="preserve">Jugendhilfe Hoffmannhaus Wilhelmsdorf</t>
   </si>
   <si>
-    <t xml:space="preserve">Stiftung Jugendhilfe aktiv</t>
+    <t xml:space="preserve">Stiftung Jugendhilfe aktiv Region Stuttgart</t>
   </si>
   <si>
     <t xml:space="preserve">Jugendhilfe Hochdorf</t>
@@ -47,7 +47,13 @@
     <t xml:space="preserve">Stiftung Tragwerk KirchheimTeck</t>
   </si>
   <si>
+    <t xml:space="preserve">Stiftung Jugendhilfe aktiv Region Böblingen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mutpol Tuttlingen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stiftung Jugendhilfe aktiv Region Esslingen</t>
   </si>
   <si>
     <t xml:space="preserve">eva Heidenheim</t>
@@ -460,7 +466,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4">
@@ -482,13 +488,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -516,7 +522,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -530,7 +536,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9">
@@ -538,13 +544,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
@@ -552,13 +558,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
@@ -566,13 +572,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -586,7 +592,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -594,13 +600,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -608,13 +614,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
@@ -622,13 +628,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C15" t="n">
         <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
@@ -636,13 +642,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -650,13 +656,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
@@ -664,13 +670,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19">
@@ -678,13 +684,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20">
@@ -692,13 +698,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>7</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21">
@@ -706,13 +712,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C21" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22">
@@ -720,13 +726,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
@@ -734,12 +740,40 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D23" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>